<commit_message>
Conclusa fase1, need fix error
</commit_message>
<xml_diff>
--- a/Documentazione/Conteggi.xlsx
+++ b/Documentazione/Conteggi.xlsx
@@ -441,8 +441,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:O22"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="O17" sqref="O17"/>
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection sqref="A1:XFD1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -485,7 +485,6 @@
     </row>
     <row r="4" spans="1:12" ht="45" customHeight="1">
       <c r="A4" s="2"/>
-      <c r="B4" s="1"/>
       <c r="C4" s="1"/>
       <c r="D4" s="1"/>
       <c r="E4" s="6" t="s">

</xml_diff>

<commit_message>
Fix index of Black
</commit_message>
<xml_diff>
--- a/Documentazione/Conteggi.xlsx
+++ b/Documentazione/Conteggi.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="18">
   <si>
     <t>O</t>
   </si>
@@ -43,13 +43,40 @@
   </si>
   <si>
     <t>mosse totali bianco</t>
+  </si>
+  <si>
+    <t>A</t>
+  </si>
+  <si>
+    <t>B</t>
+  </si>
+  <si>
+    <t>C</t>
+  </si>
+  <si>
+    <t>D</t>
+  </si>
+  <si>
+    <t>E</t>
+  </si>
+  <si>
+    <t>F</t>
+  </si>
+  <si>
+    <t>G</t>
+  </si>
+  <si>
+    <t>H</t>
+  </si>
+  <si>
+    <t>I</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+  <fonts count="4">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -60,6 +87,20 @@
     <font>
       <u/>
       <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="22"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="20"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -131,7 +172,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -145,6 +186,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normale" xfId="0" builtinId="0"/>
@@ -439,199 +482,255 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:O22"/>
+  <dimension ref="A1:P23"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection sqref="A1:XFD1"/>
+      <selection activeCell="M7" sqref="M7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="11" max="11" width="18.5703125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="18.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="45" customHeight="1">
-      <c r="A1" s="4"/>
-      <c r="B1" s="3"/>
-      <c r="C1" s="3"/>
-      <c r="D1" s="2"/>
-      <c r="E1" s="2"/>
-      <c r="F1" s="2"/>
-      <c r="G1" s="3"/>
-      <c r="H1" s="3"/>
-      <c r="I1" s="4"/>
-    </row>
-    <row r="2" spans="1:12" ht="45" customHeight="1">
-      <c r="A2" s="3"/>
-      <c r="B2" s="1"/>
-      <c r="C2" s="1"/>
-      <c r="D2" s="1"/>
+    <row r="1" spans="1:13" ht="26.25">
+      <c r="B1" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="C1" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="D1" s="12" t="s">
+        <v>11</v>
+      </c>
+      <c r="E1" s="12" t="s">
+        <v>12</v>
+      </c>
+      <c r="F1" s="12" t="s">
+        <v>13</v>
+      </c>
+      <c r="G1" s="12" t="s">
+        <v>14</v>
+      </c>
+      <c r="H1" s="12" t="s">
+        <v>15</v>
+      </c>
+      <c r="I1" s="12" t="s">
+        <v>16</v>
+      </c>
+      <c r="J1" s="12" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" ht="45" customHeight="1">
+      <c r="A2" s="11">
+        <v>0</v>
+      </c>
+      <c r="B2" s="4"/>
+      <c r="C2" s="3"/>
+      <c r="D2" s="3"/>
       <c r="E2" s="2"/>
-      <c r="F2" s="1"/>
-      <c r="G2" s="1"/>
-      <c r="H2" s="1"/>
+      <c r="F2" s="2"/>
+      <c r="G2" s="2"/>
+      <c r="H2" s="3"/>
       <c r="I2" s="3"/>
-    </row>
-    <row r="3" spans="1:12" ht="45" customHeight="1">
-      <c r="A3" s="3"/>
-      <c r="B3" s="1"/>
+      <c r="J2" s="4"/>
+    </row>
+    <row r="3" spans="1:13" ht="45" customHeight="1">
+      <c r="A3" s="11">
+        <v>1</v>
+      </c>
+      <c r="B3" s="3"/>
       <c r="C3" s="1"/>
       <c r="D3" s="1"/>
       <c r="E3" s="1"/>
-      <c r="F3" s="1"/>
+      <c r="F3" s="2"/>
       <c r="G3" s="1"/>
       <c r="H3" s="1"/>
-      <c r="I3" s="3"/>
-    </row>
-    <row r="4" spans="1:12" ht="45" customHeight="1">
-      <c r="A4" s="2"/>
+      <c r="I3" s="1"/>
+      <c r="J3" s="3"/>
+    </row>
+    <row r="4" spans="1:13" ht="45" customHeight="1">
+      <c r="A4" s="11">
+        <v>2</v>
+      </c>
+      <c r="B4" s="3"/>
       <c r="C4" s="1"/>
       <c r="D4" s="1"/>
-      <c r="E4" s="6" t="s">
-        <v>0</v>
-      </c>
+      <c r="E4" s="1"/>
       <c r="F4" s="1"/>
       <c r="G4" s="1"/>
       <c r="H4" s="1"/>
-      <c r="I4" s="2"/>
-    </row>
-    <row r="5" spans="1:12" ht="45" customHeight="1">
-      <c r="A5" s="2"/>
+      <c r="I4" s="1"/>
+      <c r="J4" s="3"/>
+    </row>
+    <row r="5" spans="1:13" ht="45" customHeight="1">
+      <c r="A5" s="11">
+        <v>3</v>
+      </c>
       <c r="B5" s="2"/>
-      <c r="C5" s="6" t="s">
-        <v>0</v>
-      </c>
-      <c r="D5" s="6" t="s">
-        <v>0</v>
-      </c>
-      <c r="E5" s="5"/>
+      <c r="D5" s="1"/>
+      <c r="E5" s="1"/>
       <c r="F5" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="G5" s="6" t="s">
+      <c r="G5" s="1"/>
+      <c r="H5" s="1"/>
+      <c r="I5" s="1"/>
+      <c r="J5" s="2"/>
+    </row>
+    <row r="6" spans="1:13" ht="45" customHeight="1">
+      <c r="A6" s="11">
+        <v>4</v>
+      </c>
+      <c r="B6" s="2"/>
+      <c r="C6" s="2"/>
+      <c r="D6" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="H5" s="2"/>
-      <c r="I5" s="2"/>
-    </row>
-    <row r="6" spans="1:12" ht="45" customHeight="1">
-      <c r="A6" s="2"/>
-      <c r="B6" s="1"/>
-      <c r="C6" s="1"/>
-      <c r="D6" s="1"/>
       <c r="E6" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="F6" s="1"/>
-      <c r="G6" s="1"/>
-      <c r="H6" s="1"/>
+      <c r="F6" s="5"/>
+      <c r="G6" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="H6" s="6" t="s">
+        <v>0</v>
+      </c>
       <c r="I6" s="2"/>
-    </row>
-    <row r="7" spans="1:12" ht="45" customHeight="1">
-      <c r="A7" s="3"/>
-      <c r="B7" s="1"/>
+      <c r="J6" s="2"/>
+    </row>
+    <row r="7" spans="1:13" ht="45" customHeight="1">
+      <c r="A7" s="11">
+        <v>5</v>
+      </c>
+      <c r="B7" s="2"/>
       <c r="C7" s="1"/>
       <c r="D7" s="1"/>
-      <c r="E7" s="6" t="s">
+      <c r="E7" s="1"/>
+      <c r="F7" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="F7" s="1"/>
       <c r="G7" s="1"/>
       <c r="H7" s="1"/>
-      <c r="I7" s="3"/>
-    </row>
-    <row r="8" spans="1:12" ht="45" customHeight="1">
-      <c r="A8" s="3"/>
-      <c r="B8" s="1"/>
+      <c r="I7" s="1"/>
+      <c r="J7" s="2"/>
+    </row>
+    <row r="8" spans="1:13" ht="45" customHeight="1">
+      <c r="A8" s="11">
+        <v>6</v>
+      </c>
+      <c r="B8" s="3"/>
       <c r="C8" s="1"/>
       <c r="D8" s="1"/>
-      <c r="E8" s="2"/>
-      <c r="F8" s="1"/>
+      <c r="E8" s="1"/>
+      <c r="F8" s="6" t="s">
+        <v>0</v>
+      </c>
       <c r="G8" s="1"/>
       <c r="H8" s="1"/>
-      <c r="I8" s="3"/>
-    </row>
-    <row r="9" spans="1:12" ht="45" customHeight="1">
-      <c r="A9" s="4"/>
+      <c r="I8" s="1"/>
+      <c r="J8" s="3"/>
+    </row>
+    <row r="9" spans="1:13" ht="45" customHeight="1">
+      <c r="A9" s="11">
+        <v>7</v>
+      </c>
       <c r="B9" s="3"/>
-      <c r="C9" s="3"/>
-      <c r="D9" s="2"/>
-      <c r="E9" s="2"/>
+      <c r="C9" s="1"/>
+      <c r="D9" s="1"/>
+      <c r="E9" s="1"/>
       <c r="F9" s="2"/>
-      <c r="G9" s="3"/>
-      <c r="H9" s="3"/>
-      <c r="I9" s="4"/>
-    </row>
-    <row r="12" spans="1:12">
-      <c r="K12" t="s">
+      <c r="G9" s="1"/>
+      <c r="H9" s="1"/>
+      <c r="I9" s="1"/>
+      <c r="J9" s="3"/>
+    </row>
+    <row r="10" spans="1:13" ht="45" customHeight="1">
+      <c r="A10" s="11">
+        <v>8</v>
+      </c>
+      <c r="B10" s="4"/>
+      <c r="C10" s="3"/>
+      <c r="D10" s="3"/>
+      <c r="E10" s="2"/>
+      <c r="F10" s="2"/>
+      <c r="G10" s="2"/>
+      <c r="H10" s="3"/>
+      <c r="I10" s="3"/>
+      <c r="J10" s="4"/>
+    </row>
+    <row r="13" spans="1:13">
+      <c r="L13" t="s">
         <v>4</v>
       </c>
-      <c r="L12">
+      <c r="M13">
         <v>81</v>
       </c>
     </row>
-    <row r="13" spans="1:12">
-      <c r="K13" t="s">
+    <row r="14" spans="1:13">
+      <c r="L14" t="s">
         <v>1</v>
       </c>
-      <c r="L13">
+      <c r="M14">
         <v>8</v>
       </c>
     </row>
-    <row r="14" spans="1:12">
-      <c r="K14" t="s">
+    <row r="15" spans="1:13">
+      <c r="L15" t="s">
         <v>2</v>
       </c>
-      <c r="L14">
+      <c r="M15">
         <v>4</v>
       </c>
     </row>
-    <row r="15" spans="1:12">
-      <c r="K15" t="s">
+    <row r="16" spans="1:13">
+      <c r="L16" t="s">
         <v>5</v>
       </c>
-      <c r="L15">
+      <c r="M16">
         <v>16</v>
       </c>
     </row>
-    <row r="16" spans="1:12">
-      <c r="K16" t="s">
+    <row r="17" spans="12:16">
+      <c r="L17" t="s">
         <v>6</v>
       </c>
-      <c r="L16" s="9">
-        <f>L13*L14*L15</f>
+      <c r="M17" s="9">
+        <f>M14*M15*M16</f>
         <v>512</v>
       </c>
     </row>
-    <row r="17" spans="11:15">
-      <c r="K17" t="s">
+    <row r="18" spans="12:16">
+      <c r="L18" t="s">
         <v>7</v>
       </c>
-      <c r="L17">
+      <c r="M18">
         <v>9</v>
       </c>
     </row>
-    <row r="18" spans="11:15">
-      <c r="K18" t="s">
+    <row r="19" spans="12:16">
+      <c r="L19" t="s">
         <v>8</v>
       </c>
-      <c r="L18" s="9">
-        <f>L13*L17</f>
+      <c r="M19" s="9">
+        <f>M14*M18</f>
         <v>72</v>
       </c>
-      <c r="M18" s="7"/>
-    </row>
-    <row r="19" spans="11:15">
-      <c r="K19" t="s">
+      <c r="N19" s="7"/>
+    </row>
+    <row r="20" spans="12:16">
+      <c r="L20" t="s">
         <v>3</v>
       </c>
-      <c r="L19" s="10">
-        <f>L13*L14</f>
+      <c r="M20" s="10">
+        <f>M14*M15</f>
         <v>32</v>
       </c>
     </row>
-    <row r="22" spans="11:15">
-      <c r="O22" s="8"/>
+    <row r="23" spans="12:16">
+      <c r="P23" s="8"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>